<commit_message>
Added pricing tab test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excelFiles/RMS_TestData.xlsx
+++ b/src/test/resources/excelFiles/RMS_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sameer\eclipse-workspace\com.axisrooms.KnightsTemplar\src\test\resources\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33E2758-B78B-4A08-801B-B51E69C224A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B59EA-D873-4EDC-81F9-BE85E34EBDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D1B72883-4199-4EB1-9BEE-D1D10B69753A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1B72883-4199-4EB1-9BEE-D1D10B69753A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="25">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>createOccupancyRule</t>
+  </si>
+  <si>
+    <t>budgetTest</t>
   </si>
 </sst>
 </file>
@@ -659,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670AFBFE-4405-4596-A4D1-35FB0F039F17}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +821,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>5</v>
@@ -828,19 +831,36 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>18</v>
+      <c r="A10" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -849,7 +869,7 @@
   <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="4" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A1048576 A1">
+  <conditionalFormatting sqref="A12:A1048576 A1">
     <cfRule type="duplicateValues" dxfId="3" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -859,11 +879,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9E35AE-6FC3-4EB7-AA4A-2B4834DB2A19}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,7 +1020,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
@@ -1017,7 +1037,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>11</v>
@@ -1030,11 +1050,11 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>18</v>
+      <c r="A10" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
@@ -1043,6 +1063,23 @@
         <v>19</v>
       </c>
       <c r="E10" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1051,10 +1088,10 @@
   <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="2" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A1048576 A1">
+  <conditionalFormatting sqref="A12:A1048576 A1">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:A1048576">
+  <conditionalFormatting sqref="A12:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="15"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"price update , reservation and sales test is added
</commit_message>
<xml_diff>
--- a/src/test/resources/excelFiles/RMS_TestData.xlsx
+++ b/src/test/resources/excelFiles/RMS_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sameer\eclipse-workspace\com.axisrooms.KnightsTemplar\src\test\resources\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55883985-8835-4D8D-8945-8954AD5E9AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761F605F-74AB-49C3-BFA2-E353C6DC1383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1B72883-4199-4EB1-9BEE-D1D10B69753A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D1B72883-4199-4EB1-9BEE-D1D10B69753A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="32">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t>optimizerTest</t>
+  </si>
+  <si>
+    <t>salesTest</t>
+  </si>
+  <si>
+    <t>salesTestForLastYearOff</t>
+  </si>
+  <si>
+    <t>salesTestForLastYearOffDownload</t>
+  </si>
+  <si>
+    <t>salesTestDownload</t>
+  </si>
+  <si>
+    <t>priceUpdateTest</t>
   </si>
 </sst>
 </file>
@@ -668,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670AFBFE-4405-4596-A4D1-35FB0F039F17}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,29 +893,114 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -909,7 +1009,7 @@
   <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="4" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A1048576 A1">
+  <conditionalFormatting sqref="A19:A1048576 A1">
     <cfRule type="duplicateValues" dxfId="3" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -919,11 +1019,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9E35AE-6FC3-4EB7-AA4A-2B4834DB2A19}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,32 +1228,117 @@
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="13" t="s">
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1162,10 +1347,10 @@
   <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="2" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A1048576 A1">
+  <conditionalFormatting sqref="A19:A1048576 A1">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A1048576">
+  <conditionalFormatting sqref="A19:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="15"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>